<commit_message>
add relative image path to readme
</commit_message>
<xml_diff>
--- a/Grid_5x5/Input/Spreadsheet/Input.xlsx
+++ b/Grid_5x5/Input/Spreadsheet/Input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\ownCloud\FOR2083\DEMONSTRATOREN\DEMONSTRATOR\_GitHub\PublicTransportNetworks\Grid_5x5\Input\Spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\ownCloud\FOR2083\DEMONSTRATOREN\DEMONSTRATOR\_GitHub\PublicTransportNetworks_Create\Grid_5x5\Input\Spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="14" r:id="rId1"/>
@@ -518,21 +518,9 @@
     <t>sum of service and empty kilometers</t>
   </si>
   <si>
-    <t>sum of service and empty hours</t>
-  </si>
-  <si>
     <t>sum of kilometers travelled for the transport of passengers</t>
   </si>
   <si>
-    <t>sum of kilometres travelled without passengers for pulling out from the depot, pulling in to the depot and interlining between two lines.</t>
-  </si>
-  <si>
-    <t>sum of hours required for the transport of passengers.</t>
-  </si>
-  <si>
-    <t>sum of hours required for pulling out, pulling in, interlining and standing at the terminal.</t>
-  </si>
-  <si>
     <t>OPERATING COST TOTAL</t>
   </si>
   <si>
@@ -543,12 +531,6 @@
   </si>
   <si>
     <t>sum of time and kilometer costs</t>
-  </si>
-  <si>
-    <t>sum of costs for personell depending on working time.</t>
-  </si>
-  <si>
-    <t>sum of costs for fuel, repair, etc. depending on kilometric performance.</t>
   </si>
   <si>
     <t>DATE OF CREATION</t>
@@ -686,7 +668,25 @@
 vehjourney situation aggregated on link level (solution)</t>
   </si>
   <si>
-    <t>05.07.2018 10:04:35</t>
+    <t>sum of kilometres travelled without passengers for pulling out from the depot, pulling in to the depot and interlining between two lines</t>
+  </si>
+  <si>
+    <t>sum of service and empty hours</t>
+  </si>
+  <si>
+    <t>sum of hours required for the transport of passengers</t>
+  </si>
+  <si>
+    <t>sum of hours required for pulling out, pulling in, interlining and standing at the terminal</t>
+  </si>
+  <si>
+    <t>sum of costs for personell depending on working time</t>
+  </si>
+  <si>
+    <t>sum of costs for fuel, repair, etc. depending on kilometric performance</t>
+  </si>
+  <si>
+    <t>06.07.2018 14:44:15</t>
   </si>
   <si>
     <t>02_Grid</t>
@@ -1731,8 +1731,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>200</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>202</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="5" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B5" s="19"/>
     </row>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B8" s="20"/>
     </row>
@@ -2005,10 +2005,10 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
@@ -2034,16 +2034,16 @@
         <v>84</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H26" s="40"/>
       <c r="I26" s="40"/>
@@ -2069,10 +2069,10 @@
         <v>41</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F27" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H27" s="40"/>
       <c r="I27" s="40"/>
@@ -2098,10 +2098,10 @@
         <v>41</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F28" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H28" s="40"/>
       <c r="I28" s="40"/>
@@ -2127,10 +2127,10 @@
         <v>41</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H29" s="40"/>
       <c r="I29" s="40"/>
@@ -2156,10 +2156,10 @@
         <v>40</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H30" s="40"/>
       <c r="I30" s="40"/>
@@ -2178,17 +2178,17 @@
         <v>142</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C31" s="34"/>
       <c r="D31" s="22" t="s">
         <v>40</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F31" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H31" s="40"/>
       <c r="I31" s="40"/>
@@ -2207,17 +2207,17 @@
         <v>143</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>150</v>
+        <v>194</v>
       </c>
       <c r="C32" s="34"/>
       <c r="D32" s="22" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F32" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H32" s="40"/>
       <c r="I32" s="40"/>
@@ -2236,17 +2236,17 @@
         <v>145</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>148</v>
+        <v>195</v>
       </c>
       <c r="C33" s="34"/>
       <c r="D33" s="22" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F33" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2254,17 +2254,17 @@
         <v>144</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
       <c r="C34" s="34"/>
       <c r="D34" s="22" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F34" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2272,162 +2272,162 @@
         <v>146</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
       <c r="C35" s="34"/>
       <c r="D35" s="22" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F35" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C36" s="36"/>
       <c r="D36" s="22" t="s">
         <v>123</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F36" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="C37" s="36"/>
       <c r="D37" s="22" t="s">
         <v>123</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F37" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>158</v>
+        <v>199</v>
       </c>
       <c r="C38" s="36"/>
       <c r="D38" s="22" t="s">
         <v>123</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F38" s="41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C39" s="37"/>
       <c r="D39" s="22" t="s">
         <v>124</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F39" s="41" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C40" s="38"/>
       <c r="D40" s="22" t="s">
         <v>124</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F40" s="41" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C41" s="38"/>
       <c r="D41" s="22" t="s">
         <v>41</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F41" s="41" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G41" s="23"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C42" s="38"/>
       <c r="D42" s="22" t="s">
         <v>41</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F42" s="41" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C43" s="39"/>
       <c r="D43" s="62" t="s">
         <v>41</v>
       </c>
       <c r="E43" s="63" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F43" s="64" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2675,10 +2675,10 @@
         <v>28</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D13" s="49" t="s">
         <v>41</v>
@@ -2695,10 +2695,10 @@
         <v>28</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D14" s="49" t="s">
         <v>41</v>
@@ -2713,10 +2713,10 @@
         <v>28</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D15" s="49" t="s">
         <v>41</v>
@@ -2983,7 +2983,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D28" s="49" t="s">
         <v>41</v>
@@ -3002,7 +3002,7 @@
         <v>50</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D29" s="49" t="s">
         <v>41</v>
@@ -3020,7 +3020,7 @@
         <v>51</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D30" s="49" t="s">
         <v>41</v>
@@ -3038,7 +3038,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="52" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D31" s="49" t="s">
         <v>41</v>
@@ -3125,7 +3125,7 @@
         <v>62</v>
       </c>
       <c r="C36" s="53" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D36" s="49" t="s">
         <v>41</v>
@@ -3142,7 +3142,7 @@
         <v>8</v>
       </c>
       <c r="C37" s="53" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D37" s="49" t="s">
         <v>41</v>
@@ -3204,13 +3204,13 @@
     </row>
     <row r="41" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="47" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B41" s="54" t="s">
         <v>62</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D41" s="49" t="s">
         <v>41</v>
@@ -3221,13 +3221,13 @@
     </row>
     <row r="42" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="47" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B42" s="54" t="s">
         <v>59</v>
       </c>
       <c r="C42" s="53" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D42" s="49" t="s">
         <v>41</v>
@@ -3238,7 +3238,7 @@
     </row>
     <row r="43" spans="1:5" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="47" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B43" s="54" t="s">
         <v>57</v>
@@ -3255,7 +3255,7 @@
     </row>
     <row r="44" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="47" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B44" s="54" t="s">
         <v>23</v>
@@ -3272,13 +3272,13 @@
     </row>
     <row r="45" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="47" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B45" s="54" t="s">
         <v>60</v>
       </c>
       <c r="C45" s="53" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D45" s="49" t="s">
         <v>41</v>
@@ -3289,13 +3289,13 @@
     </row>
     <row r="46" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="47" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B46" s="54" t="s">
         <v>61</v>
       </c>
       <c r="C46" s="53" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D46" s="49" t="s">
         <v>40</v>
@@ -3344,7 +3344,7 @@
         <v>59</v>
       </c>
       <c r="C49" s="53" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D49" s="55"/>
       <c r="E49" s="49" t="s">
@@ -6998,16 +6998,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="66" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D4" s="66" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E4" s="66" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F4" s="66" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -19541,7 +19541,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:H25"/>
     </sheetView>
   </sheetViews>
@@ -19555,7 +19555,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="72" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -19808,7 +19808,7 @@
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="72" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B27" s="73"/>
       <c r="C27" s="73"/>
@@ -20070,7 +20070,7 @@
     </row>
     <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="72" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B53" s="73"/>
       <c r="C53" s="73"/>

</xml_diff>